<commit_message>
Added usage examples for worksheet operations
- Add examples for inserting images into worksheets.
- Demonstrate how to extract images from worksheets.
- Show how to remove a worksheet by name with verification of removal.

The commit enriches the documentation with practical usage examples for image handling and worksheet management in the FileFormat.Cells.Examples project, providing users with clear guidance on applying these operations.
</commit_message>
<xml_diff>
--- a/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
+++ b/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7f48aa6cfe454ada"/>
-    <x:sheet name="NewWorksheet" sheetId="2" r:id="Rc93d6b4b8a724a21"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R243ac593c01a4d34"/>
+    <x:sheet name="NewWorksheet" sheetId="2" r:id="R086a0d37f7c8407a"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
feat: Add example for setting values in worksheet range
Add a new method `SetRangeValue` to the `WorksheetExamples` class, demonstrating how to select a range within an Excel worksheet and uniformly set values across all cells in the range. This example includes loading the workbook, selecting the range, setting the value, and saving the changes, complete with console output for verification.

This enhancement enriches the FileFormat.Cells.Examples with practical guidance on manipulating cell ranges, catering to common use cases in Excel file processing.
</commit_message>
<xml_diff>
--- a/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
+++ b/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R243ac593c01a4d34"/>
-    <x:sheet name="NewWorksheet" sheetId="2" r:id="R086a0d37f7c8407a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R906edbf7d01e4f02"/>
+    <x:sheet name="NewWorksheet" sheetId="2" r:id="Re55d016d21074f50"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
feat: Add method for inserting rows in a worksheet
Introduce `InsertRowsIntoWorksheet` in the WorksheetExamples class to illustrate how to insert multiple rows into a specific position within an Excel worksheet. The example demonstrates loading a workbook, identifying the target worksheet, inserting rows, and saving the workbook with updated content. Includes console output to verify the operation's success.
</commit_message>
<xml_diff>
--- a/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
+++ b/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R906edbf7d01e4f02"/>
-    <x:sheet name="NewWorksheet" sheetId="2" r:id="Re55d016d21074f50"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R3a860c5a6ef74426"/>
+    <x:sheet name="NewWorksheet" sheetId="2" r:id="Rf926a3737cba44f2"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
feat: Add method for inserting columns in a worksheet
Implement `InsertColumnsIntoWorksheet` within the WorksheetExamples class, providing a clear example of how to add columns to an Excel worksheet at a specific position. The example details the steps for loading the workbook, selecting the appropriate worksheet, inserting columns, and saving the workbook, along with console output for immediate feedback on the operation's result.
</commit_message>
<xml_diff>
--- a/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
+++ b/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R3a860c5a6ef74426"/>
-    <x:sheet name="NewWorksheet" sheetId="2" r:id="Rf926a3737cba44f2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbd28a1fb48e34ccd"/>
+    <x:sheet name="NewWorksheet" sheetId="2" r:id="Rf9f8f1942b1547bd"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
docs: Add example code for using FreezePane method in Worksheet
- Added a new example demonstrating how to use the FreezePane method within the Worksheet class.
- Example showcases setting frozen rows and columns to improve usability and clarify method usage.
</commit_message>
<xml_diff>
--- a/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
+++ b/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbd28a1fb48e34ccd"/>
-    <x:sheet name="NewWorksheet" sheetId="2" r:id="Rf9f8f1942b1547bd"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re4d2d4af09564c8e"/>
+    <x:sheet name="NewWorksheet" sheetId="2" r:id="Rf2e77b2314704bf0"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
Upgraded to Open XML 3.2.0 and upgrade to FileFormat.Cells.25.1.0
</commit_message>
<xml_diff>
--- a/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
+++ b/FileFormat.Cells.Examples.Usage/spreadSheetDocuments/Workbook/spreadsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re4d2d4af09564c8e"/>
-    <x:sheet name="NewWorksheet" sheetId="2" r:id="Rf2e77b2314704bf0"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6a7a0e3ea8c44966"/>
+    <x:sheet name="NewWorksheet" sheetId="2" r:id="R93b9ee2ab7d44afc"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>